<commit_message>
Changes to UX folder
</commit_message>
<xml_diff>
--- a/UX Design/User Feedback/News Headline Matching Website Survey (Responses).xlsx
+++ b/UX Design/User Feedback/News Headline Matching Website Survey (Responses).xlsx
@@ -5,21 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillip/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillip/Documents/UoB_group_project/UX Design/User Feedback/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B3DEA3-E81A-B34C-A84A-9F9B1DAF9D52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21F6ADD-34CA-9149-BA4D-35BE1446CD2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$19:$C$19</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$A$20:$C$20</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -378,6 +374,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5070-8C40-9342-E1A63A71982D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -393,6 +394,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5070-8C40-9342-E1A63A71982D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -408,6 +414,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5070-8C40-9342-E1A63A71982D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -423,6 +434,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5070-8C40-9342-E1A63A71982D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -438,10 +454,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-5070-8C40-9342-E1A63A71982D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$E$1</c:f>
+              <c:f>Graphs!$A$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -464,7 +485,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$E$2</c:f>
+              <c:f>Graphs!$A$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -670,6 +691,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9030-2448-9B50-78C249A733DA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -685,6 +711,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-9030-2448-9B50-78C249A733DA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -700,10 +731,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-9030-2448-9B50-78C249A733DA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$7:$C$7</c:f>
+              <c:f>Graphs!$A$7:$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -720,7 +756,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$8:$C$8</c:f>
+              <c:f>Graphs!$A$8:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -920,6 +956,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-577F-D247-A28E-8BD240AFD7CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -935,10 +976,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-577F-D247-A28E-8BD240AFD7CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$13:$B$13</c:f>
+              <c:f>Graphs!$A$13:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -952,7 +998,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$B$14</c:f>
+              <c:f>Graphs!$A$14:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1094,6 +1140,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7B14-8241-BC95-307930B65FA7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1109,6 +1160,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7B14-8241-BC95-307930B65FA7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1124,10 +1180,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7B14-8241-BC95-307930B65FA7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$19:$C$19</c:f>
+              <c:f>Graphs!$A$19:$C$19</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1144,7 +1205,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$20:$C$20</c:f>
+              <c:f>Graphs!$A$20:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3841,7 +3902,7 @@
   </sheetPr>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
@@ -4392,7 +4453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8076FB98-614A-1F41-BE30-2CEE78BDFA86}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C20" sqref="A19:C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>